<commit_message>
atualizando com o excel classificado
</commit_message>
<xml_diff>
--- a/volkswagen.xlsx
+++ b/volkswagen.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dudup\Documents\CDADOS21\P1-2021-Cdados-2A\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/660d30a862cc4521/Documentos/2021.1/Ciencia dos Dados 2A/Projeto 1/P1-2021-Cdados-3A/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E085274-12E0-4060-AF84-3EDC0976F1CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="339" documentId="13_ncr:1_{9660DD74-61A9-F140-AD3D-CD87F626FD90}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{A227986C-F5B4-4AA6-A6B4-4C3BB875148A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -1868,7 +1868,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1876,6 +1876,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -2217,8 +2219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N301"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2239,7 +2241,7 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="6">
         <v>0</v>
       </c>
     </row>
@@ -2248,7 +2250,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2264,7 +2266,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2280,7 +2282,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -2288,7 +2290,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -2296,7 +2298,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -2312,7 +2314,7 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -2336,7 +2338,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -2352,7 +2354,7 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -2360,7 +2362,7 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -2392,7 +2394,7 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -2400,7 +2402,7 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -2408,7 +2410,7 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -2432,7 +2434,7 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -2448,7 +2450,7 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -2472,7 +2474,7 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -2509,7 +2511,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -2549,7 +2551,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -2557,7 +2559,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -2565,7 +2567,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -2605,7 +2607,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -2653,7 +2655,7 @@
         <v>52</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -2661,7 +2663,7 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -2677,7 +2679,7 @@
         <v>55</v>
       </c>
       <c r="B57">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -2685,7 +2687,7 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -2693,7 +2695,7 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -2701,7 +2703,7 @@
         <v>58</v>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -2757,7 +2759,7 @@
         <v>65</v>
       </c>
       <c r="B67">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -2789,7 +2791,7 @@
         <v>69</v>
       </c>
       <c r="B71">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -2813,7 +2815,7 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -2821,7 +2823,7 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -2845,7 +2847,7 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -2853,7 +2855,7 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -2869,7 +2871,7 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -2909,7 +2911,7 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -2917,7 +2919,7 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -2933,7 +2935,7 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
@@ -2941,7 +2943,7 @@
         <v>88</v>
       </c>
       <c r="B90">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
@@ -2957,7 +2959,7 @@
         <v>90</v>
       </c>
       <c r="B92">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
@@ -2965,7 +2967,7 @@
         <v>91</v>
       </c>
       <c r="B93">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
@@ -3013,7 +3015,7 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.3">
@@ -3053,7 +3055,7 @@
         <v>102</v>
       </c>
       <c r="B104">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.3">
@@ -3061,7 +3063,7 @@
         <v>103</v>
       </c>
       <c r="B105">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.3">
@@ -3069,7 +3071,7 @@
         <v>104</v>
       </c>
       <c r="B106">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.3">
@@ -3077,7 +3079,7 @@
         <v>105</v>
       </c>
       <c r="B107">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.3">
@@ -3110,7 +3112,7 @@
         <v>109</v>
       </c>
       <c r="B111">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.3">
@@ -3134,7 +3136,7 @@
         <v>112</v>
       </c>
       <c r="B114">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
@@ -3166,7 +3168,7 @@
         <v>116</v>
       </c>
       <c r="B118">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.3">
@@ -3198,7 +3200,7 @@
         <v>120</v>
       </c>
       <c r="B122">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.3">
@@ -3246,7 +3248,7 @@
         <v>126</v>
       </c>
       <c r="B128">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.3">
@@ -3310,7 +3312,7 @@
         <v>134</v>
       </c>
       <c r="B136">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.3">
@@ -3334,7 +3336,7 @@
         <v>137</v>
       </c>
       <c r="B139">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.3">
@@ -3366,7 +3368,7 @@
         <v>141</v>
       </c>
       <c r="B143">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.3">
@@ -3374,7 +3376,7 @@
         <v>142</v>
       </c>
       <c r="B144">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
@@ -3406,7 +3408,7 @@
         <v>146</v>
       </c>
       <c r="B148">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
@@ -3422,7 +3424,7 @@
         <v>148</v>
       </c>
       <c r="B150">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
@@ -3430,7 +3432,7 @@
         <v>149</v>
       </c>
       <c r="B151" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
@@ -3446,7 +3448,7 @@
         <v>151</v>
       </c>
       <c r="B153">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
@@ -3486,7 +3488,7 @@
         <v>156</v>
       </c>
       <c r="B158">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
@@ -3494,7 +3496,7 @@
         <v>157</v>
       </c>
       <c r="B159">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
@@ -3502,7 +3504,7 @@
         <v>158</v>
       </c>
       <c r="B160">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
@@ -3510,7 +3512,7 @@
         <v>159</v>
       </c>
       <c r="B161">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
@@ -3518,7 +3520,7 @@
         <v>160</v>
       </c>
       <c r="B162">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
@@ -3526,7 +3528,7 @@
         <v>161</v>
       </c>
       <c r="B163">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
@@ -3566,7 +3568,7 @@
         <v>166</v>
       </c>
       <c r="B168">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
@@ -3582,7 +3584,7 @@
         <v>168</v>
       </c>
       <c r="B170">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
@@ -3590,7 +3592,7 @@
         <v>169</v>
       </c>
       <c r="B171">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
@@ -3638,7 +3640,7 @@
         <v>175</v>
       </c>
       <c r="B177">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
@@ -3710,7 +3712,7 @@
         <v>184</v>
       </c>
       <c r="B186">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
@@ -3758,7 +3760,7 @@
         <v>190</v>
       </c>
       <c r="B192">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
@@ -3798,7 +3800,7 @@
         <v>195</v>
       </c>
       <c r="B197">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
@@ -3846,7 +3848,7 @@
         <v>201</v>
       </c>
       <c r="B203">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
@@ -3854,7 +3856,7 @@
         <v>202</v>
       </c>
       <c r="B204">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
@@ -3878,7 +3880,7 @@
         <v>205</v>
       </c>
       <c r="B207">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
@@ -3926,7 +3928,7 @@
         <v>211</v>
       </c>
       <c r="B213">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
@@ -3942,7 +3944,7 @@
         <v>213</v>
       </c>
       <c r="B215">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
@@ -3950,7 +3952,7 @@
         <v>214</v>
       </c>
       <c r="B216">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
@@ -3974,7 +3976,7 @@
         <v>217</v>
       </c>
       <c r="B219">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
@@ -3998,7 +4000,7 @@
         <v>220</v>
       </c>
       <c r="B222">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
@@ -4006,7 +4008,7 @@
         <v>221</v>
       </c>
       <c r="B223">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
@@ -4022,7 +4024,7 @@
         <v>223</v>
       </c>
       <c r="B225">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
@@ -4070,7 +4072,7 @@
         <v>229</v>
       </c>
       <c r="B231">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
@@ -4078,7 +4080,7 @@
         <v>230</v>
       </c>
       <c r="B232">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
@@ -4086,7 +4088,7 @@
         <v>231</v>
       </c>
       <c r="B233">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
@@ -4110,7 +4112,7 @@
         <v>234</v>
       </c>
       <c r="B236">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
@@ -4118,7 +4120,7 @@
         <v>235</v>
       </c>
       <c r="B237">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
@@ -4134,7 +4136,7 @@
         <v>237</v>
       </c>
       <c r="B239">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
@@ -4158,7 +4160,7 @@
         <v>240</v>
       </c>
       <c r="B242">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
@@ -4166,7 +4168,7 @@
         <v>241</v>
       </c>
       <c r="B243">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
@@ -4222,7 +4224,7 @@
         <v>248</v>
       </c>
       <c r="B250">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
@@ -4230,7 +4232,7 @@
         <v>249</v>
       </c>
       <c r="B251">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
@@ -4286,7 +4288,7 @@
         <v>256</v>
       </c>
       <c r="B258">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
@@ -4294,7 +4296,7 @@
         <v>257</v>
       </c>
       <c r="B259">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
@@ -4318,7 +4320,7 @@
         <v>260</v>
       </c>
       <c r="B262">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
@@ -4414,7 +4416,7 @@
         <v>272</v>
       </c>
       <c r="B274">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
@@ -4422,7 +4424,7 @@
         <v>273</v>
       </c>
       <c r="B275">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
@@ -4430,7 +4432,7 @@
         <v>274</v>
       </c>
       <c r="B276">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
@@ -4478,7 +4480,7 @@
         <v>280</v>
       </c>
       <c r="B282">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
@@ -4494,7 +4496,7 @@
         <v>282</v>
       </c>
       <c r="B284">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
@@ -4502,7 +4504,7 @@
         <v>283</v>
       </c>
       <c r="B285">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
@@ -4534,7 +4536,7 @@
         <v>287</v>
       </c>
       <c r="B289">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
@@ -4558,7 +4560,7 @@
         <v>290</v>
       </c>
       <c r="B292">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
@@ -4566,7 +4568,7 @@
         <v>291</v>
       </c>
       <c r="B293">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
@@ -4582,7 +4584,7 @@
         <v>293</v>
       </c>
       <c r="B295">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
@@ -4590,7 +4592,7 @@
         <v>294</v>
       </c>
       <c r="B296">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
@@ -4598,7 +4600,7 @@
         <v>295</v>
       </c>
       <c r="B297">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
@@ -4646,8 +4648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B108" sqref="B108"/>
+    <sheetView zoomScale="64" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="A138" sqref="A138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4659,7 +4661,7 @@
       <c r="A1" s="1" t="s">
         <v>300</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>501</v>
       </c>
     </row>
@@ -4667,7 +4669,7 @@
       <c r="A2" t="s">
         <v>301</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4675,7 +4677,7 @@
       <c r="A3" t="s">
         <v>302</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4683,7 +4685,7 @@
       <c r="A4" t="s">
         <v>303</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>3</v>
       </c>
     </row>
@@ -4691,7 +4693,7 @@
       <c r="A5" t="s">
         <v>304</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>1</v>
       </c>
     </row>
@@ -4699,7 +4701,7 @@
       <c r="A6" t="s">
         <v>305</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="5">
         <v>2</v>
       </c>
     </row>
@@ -4707,7 +4709,7 @@
       <c r="A7" t="s">
         <v>306</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="5">
         <v>2</v>
       </c>
     </row>
@@ -4715,7 +4717,7 @@
       <c r="A8" t="s">
         <v>307</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <v>1</v>
       </c>
     </row>
@@ -4723,7 +4725,7 @@
       <c r="A9" t="s">
         <v>308</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <v>1</v>
       </c>
     </row>
@@ -4731,7 +4733,7 @@
       <c r="A10" t="s">
         <v>309</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4739,7 +4741,7 @@
       <c r="A11" t="s">
         <v>310</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4747,7 +4749,7 @@
       <c r="A12" t="s">
         <v>311</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4755,7 +4757,7 @@
       <c r="A13" t="s">
         <v>312</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="5">
         <v>1</v>
       </c>
     </row>
@@ -4763,7 +4765,7 @@
       <c r="A14" t="s">
         <v>313</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="5">
         <v>1</v>
       </c>
     </row>
@@ -4771,7 +4773,7 @@
       <c r="A15" t="s">
         <v>314</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="5">
         <v>2</v>
       </c>
     </row>
@@ -4779,7 +4781,7 @@
       <c r="A16" t="s">
         <v>315</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="5">
         <v>2</v>
       </c>
     </row>
@@ -4787,7 +4789,7 @@
       <c r="A17" t="s">
         <v>316</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="5">
         <v>3</v>
       </c>
     </row>
@@ -4795,7 +4797,7 @@
       <c r="A18" t="s">
         <v>317</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="5">
         <v>3</v>
       </c>
     </row>
@@ -4803,7 +4805,7 @@
       <c r="A19" t="s">
         <v>318</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="5">
         <v>2</v>
       </c>
     </row>
@@ -4811,7 +4813,7 @@
       <c r="A20" t="s">
         <v>319</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="5">
         <v>3</v>
       </c>
     </row>
@@ -4819,7 +4821,7 @@
       <c r="A21" t="s">
         <v>320</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4827,7 +4829,7 @@
       <c r="A22" t="s">
         <v>321</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="5">
         <v>3</v>
       </c>
     </row>
@@ -4835,7 +4837,7 @@
       <c r="A23" t="s">
         <v>322</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="5">
         <v>3</v>
       </c>
     </row>
@@ -4843,7 +4845,7 @@
       <c r="A24" t="s">
         <v>323</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="5">
         <v>2</v>
       </c>
     </row>
@@ -4851,7 +4853,7 @@
       <c r="A25" t="s">
         <v>324</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="5">
         <v>2</v>
       </c>
     </row>
@@ -4859,7 +4861,7 @@
       <c r="A26" t="s">
         <v>325</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="5">
         <v>3</v>
       </c>
     </row>
@@ -4867,7 +4869,7 @@
       <c r="A27" t="s">
         <v>326</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="5">
         <v>3</v>
       </c>
     </row>
@@ -4875,7 +4877,7 @@
       <c r="A28" t="s">
         <v>327</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="5">
         <v>3</v>
       </c>
     </row>
@@ -4883,7 +4885,7 @@
       <c r="A29" t="s">
         <v>328</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="5">
         <v>3</v>
       </c>
     </row>
@@ -4891,7 +4893,7 @@
       <c r="A30" t="s">
         <v>329</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="5">
         <v>1</v>
       </c>
     </row>
@@ -4899,7 +4901,7 @@
       <c r="A31" t="s">
         <v>330</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="5">
         <v>1</v>
       </c>
     </row>
@@ -4907,7 +4909,7 @@
       <c r="A32" t="s">
         <v>331</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="5">
         <v>3</v>
       </c>
     </row>
@@ -4915,7 +4917,7 @@
       <c r="A33" t="s">
         <v>332</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4923,7 +4925,7 @@
       <c r="A34" t="s">
         <v>333</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="5">
         <v>1</v>
       </c>
     </row>
@@ -4931,7 +4933,7 @@
       <c r="A35" t="s">
         <v>334</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="5">
         <v>1</v>
       </c>
     </row>
@@ -4939,7 +4941,7 @@
       <c r="A36" t="s">
         <v>335</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4947,7 +4949,7 @@
       <c r="A37" t="s">
         <v>336</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="5">
         <v>2</v>
       </c>
     </row>
@@ -4955,7 +4957,7 @@
       <c r="A38" t="s">
         <v>337</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="5">
         <v>2</v>
       </c>
     </row>
@@ -4963,7 +4965,7 @@
       <c r="A39" t="s">
         <v>338</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="5">
         <v>2</v>
       </c>
     </row>
@@ -4971,7 +4973,7 @@
       <c r="A40" t="s">
         <v>339</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="5">
         <v>2</v>
       </c>
     </row>
@@ -4979,7 +4981,7 @@
       <c r="A41" t="s">
         <v>340</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4987,7 +4989,7 @@
       <c r="A42" t="s">
         <v>341</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="5">
         <v>3</v>
       </c>
     </row>
@@ -4995,7 +4997,7 @@
       <c r="A43" t="s">
         <v>342</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="5">
         <v>0</v>
       </c>
     </row>
@@ -5003,7 +5005,7 @@
       <c r="A44" t="s">
         <v>343</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5011,7 +5013,7 @@
       <c r="A45" t="s">
         <v>344</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="5">
         <v>2</v>
       </c>
     </row>
@@ -5019,7 +5021,7 @@
       <c r="A46" t="s">
         <v>345</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5027,7 +5029,7 @@
       <c r="A47" t="s">
         <v>346</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5035,7 +5037,7 @@
       <c r="A48" t="s">
         <v>347</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="5">
         <v>3</v>
       </c>
     </row>
@@ -5043,7 +5045,7 @@
       <c r="A49" t="s">
         <v>348</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5051,7 +5053,7 @@
       <c r="A50" t="s">
         <v>349</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="5">
         <v>3</v>
       </c>
     </row>
@@ -5059,7 +5061,7 @@
       <c r="A51" t="s">
         <v>350</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="5">
         <v>0</v>
       </c>
     </row>
@@ -5067,7 +5069,7 @@
       <c r="A52" t="s">
         <v>351</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="5">
         <v>3</v>
       </c>
     </row>
@@ -5075,7 +5077,7 @@
       <c r="A53" t="s">
         <v>352</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="5">
         <v>2</v>
       </c>
     </row>
@@ -5083,7 +5085,7 @@
       <c r="A54" t="s">
         <v>353</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="5">
         <v>3</v>
       </c>
     </row>
@@ -5091,7 +5093,7 @@
       <c r="A55" t="s">
         <v>354</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="5">
         <v>0</v>
       </c>
     </row>
@@ -5099,7 +5101,7 @@
       <c r="A56" t="s">
         <v>355</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="5">
         <v>0</v>
       </c>
     </row>
@@ -5107,7 +5109,7 @@
       <c r="A57" t="s">
         <v>356</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="5">
         <v>3</v>
       </c>
     </row>
@@ -5115,7 +5117,7 @@
       <c r="A58" t="s">
         <v>357</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="5">
         <v>2</v>
       </c>
     </row>
@@ -5123,7 +5125,7 @@
       <c r="A59" t="s">
         <v>358</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5131,7 +5133,7 @@
       <c r="A60" t="s">
         <v>359</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="5">
         <v>2</v>
       </c>
     </row>
@@ -5139,7 +5141,7 @@
       <c r="A61" t="s">
         <v>360</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="5">
         <v>3</v>
       </c>
     </row>
@@ -5147,7 +5149,7 @@
       <c r="A62" t="s">
         <v>361</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5155,7 +5157,7 @@
       <c r="A63" t="s">
         <v>362</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="5">
         <v>3</v>
       </c>
     </row>
@@ -5163,7 +5165,7 @@
       <c r="A64" t="s">
         <v>363</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="5">
         <v>2</v>
       </c>
     </row>
@@ -5171,7 +5173,7 @@
       <c r="A65" t="s">
         <v>364</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="5">
         <v>2</v>
       </c>
     </row>
@@ -5179,7 +5181,7 @@
       <c r="A66" t="s">
         <v>365</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="5">
         <v>3</v>
       </c>
     </row>
@@ -5187,7 +5189,7 @@
       <c r="A67" t="s">
         <v>366</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5195,7 +5197,7 @@
       <c r="A68" t="s">
         <v>367</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="5">
         <v>0</v>
       </c>
     </row>
@@ -5203,7 +5205,7 @@
       <c r="A69" t="s">
         <v>368</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5211,7 +5213,7 @@
       <c r="A70" t="s">
         <v>369</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="5">
         <v>3</v>
       </c>
     </row>
@@ -5219,7 +5221,7 @@
       <c r="A71" t="s">
         <v>370</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5227,7 +5229,7 @@
       <c r="A72" t="s">
         <v>371</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5235,7 +5237,7 @@
       <c r="A73" t="s">
         <v>372</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="5">
         <v>2</v>
       </c>
     </row>
@@ -5243,7 +5245,7 @@
       <c r="A74" t="s">
         <v>373</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5251,7 +5253,7 @@
       <c r="A75" t="s">
         <v>374</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="5">
         <v>3</v>
       </c>
     </row>
@@ -5259,7 +5261,7 @@
       <c r="A76" t="s">
         <v>375</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="5">
         <v>2</v>
       </c>
     </row>
@@ -5267,7 +5269,7 @@
       <c r="A77" t="s">
         <v>376</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="5">
         <v>3</v>
       </c>
     </row>
@@ -5275,7 +5277,7 @@
       <c r="A78" t="s">
         <v>377</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5283,7 +5285,7 @@
       <c r="A79" t="s">
         <v>378</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5291,7 +5293,7 @@
       <c r="A80" t="s">
         <v>379</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="5">
         <v>3</v>
       </c>
     </row>
@@ -5299,7 +5301,7 @@
       <c r="A81" t="s">
         <v>380</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="5">
         <v>0</v>
       </c>
     </row>
@@ -5307,7 +5309,7 @@
       <c r="A82" t="s">
         <v>381</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5315,7 +5317,7 @@
       <c r="A83" t="s">
         <v>382</v>
       </c>
-      <c r="B83">
+      <c r="B83" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5323,7 +5325,7 @@
       <c r="A84" t="s">
         <v>383</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5331,7 +5333,7 @@
       <c r="A85" t="s">
         <v>384</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5339,7 +5341,7 @@
       <c r="A86" t="s">
         <v>385</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="5">
         <v>2</v>
       </c>
     </row>
@@ -5347,7 +5349,7 @@
       <c r="A87" t="s">
         <v>386</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5355,7 +5357,7 @@
       <c r="A88" t="s">
         <v>387</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="5">
         <v>0</v>
       </c>
     </row>
@@ -5363,7 +5365,7 @@
       <c r="A89" t="s">
         <v>388</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="5">
         <v>3</v>
       </c>
     </row>
@@ -5371,7 +5373,7 @@
       <c r="A90" t="s">
         <v>389</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="5">
         <v>2</v>
       </c>
     </row>
@@ -5379,7 +5381,7 @@
       <c r="A91" t="s">
         <v>390</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5387,7 +5389,7 @@
       <c r="A92" t="s">
         <v>391</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="5">
         <v>2</v>
       </c>
     </row>
@@ -5395,7 +5397,7 @@
       <c r="A93" t="s">
         <v>392</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="5">
         <v>0</v>
       </c>
     </row>
@@ -5403,7 +5405,7 @@
       <c r="A94" t="s">
         <v>393</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="5">
         <v>0</v>
       </c>
     </row>
@@ -5411,7 +5413,7 @@
       <c r="A95" t="s">
         <v>394</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="5">
         <v>3</v>
       </c>
     </row>
@@ -5419,7 +5421,7 @@
       <c r="A96" t="s">
         <v>395</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5427,7 +5429,7 @@
       <c r="A97" t="s">
         <v>396</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="5">
         <v>0</v>
       </c>
     </row>
@@ -5435,7 +5437,7 @@
       <c r="A98" t="s">
         <v>397</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="5">
         <v>0</v>
       </c>
     </row>
@@ -5443,7 +5445,7 @@
       <c r="A99" t="s">
         <v>398</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="5">
         <v>0</v>
       </c>
     </row>
@@ -5451,7 +5453,7 @@
       <c r="A100" t="s">
         <v>399</v>
       </c>
-      <c r="B100">
+      <c r="B100" s="5">
         <v>0</v>
       </c>
     </row>
@@ -5459,7 +5461,7 @@
       <c r="A101" t="s">
         <v>400</v>
       </c>
-      <c r="B101">
+      <c r="B101" s="5">
         <v>3</v>
       </c>
     </row>
@@ -5467,7 +5469,7 @@
       <c r="A102" t="s">
         <v>401</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5475,7 +5477,7 @@
       <c r="A103" t="s">
         <v>402</v>
       </c>
-      <c r="B103">
+      <c r="B103" s="5">
         <v>2</v>
       </c>
     </row>
@@ -5483,7 +5485,7 @@
       <c r="A104" t="s">
         <v>403</v>
       </c>
-      <c r="B104">
+      <c r="B104" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5491,7 +5493,7 @@
       <c r="A105" t="s">
         <v>404</v>
       </c>
-      <c r="B105">
+      <c r="B105" s="5">
         <v>0</v>
       </c>
     </row>
@@ -5499,7 +5501,7 @@
       <c r="A106" t="s">
         <v>405</v>
       </c>
-      <c r="B106">
+      <c r="B106" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5507,7 +5509,7 @@
       <c r="A107" t="s">
         <v>406</v>
       </c>
-      <c r="B107">
+      <c r="B107" s="5">
         <v>1</v>
       </c>
     </row>
@@ -5515,470 +5517,752 @@
       <c r="A108" t="s">
         <v>407</v>
       </c>
+      <c r="B108" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>408</v>
       </c>
+      <c r="B109" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>409</v>
       </c>
+      <c r="B110" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>410</v>
       </c>
+      <c r="B111" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B112" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B113" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B114" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B115" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B116" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B117" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>417</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B118" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B119" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B120" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B121" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B122" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B123" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B124" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B125" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B126" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B127" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B128" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B129" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B130" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B131" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B132" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B133" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B134" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B135" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B136" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B137" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B138" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B139" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B140" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B141" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B142" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B143" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B144" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B145" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B146" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B147" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B148" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B149" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B150" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B151" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B152" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B153" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B154" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B155" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B156" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>456</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B157" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>457</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B158" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>458</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B159" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B160" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>460</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B161" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>461</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B162" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>462</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B163" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>463</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B164" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>464</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B165" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B166" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>466</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B167" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>467</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B168" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>468</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B169" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>469</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B170" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>470</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B171" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>471</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B172" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B173" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>473</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B174" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>474</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B175" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>475</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B176" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>476</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B177" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B178" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>478</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B179" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B180" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B181" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>481</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B182" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>482</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B183" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B184" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B185" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B186" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B187" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>487</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B188" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>488</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B189" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>489</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B190" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>490</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B191" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B192" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B193" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>493</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B194" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>494</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B195" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>495</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B196" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B197" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B198" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B199" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B200" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>500</v>
+      </c>
+      <c r="B201" s="5">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>